<commit_message>
Adjusted threshold slightly for better results
Not much left to do on this project!
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -3,14 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909B9759-C74F-4055-BA1E-E0CEE18B67C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D984F5-3BB6-49D1-80D7-B9479A0364DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c0.6322369" sheetId="1" r:id="rId1"/>
+    <sheet name="HotNewC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
   <si>
     <t>Accuracy</t>
   </si>
@@ -437,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -897,6 +899,513 @@
       <c r="I19">
         <f t="shared" si="7"/>
         <v>0.99818341896153895</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:D13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:I13">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:I11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCFA4DA-2F81-4370-BEFA-BFE35C1005F5}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.92171428571428504</v>
+      </c>
+      <c r="C3">
+        <v>0.64718797069260403</v>
+      </c>
+      <c r="D3">
+        <v>0.94969414225832505</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3">
+        <v>0.93203541912632804</v>
+      </c>
+      <c r="H3">
+        <v>0.73907887953256501</v>
+      </c>
+      <c r="I3">
+        <v>0.96277134488516602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.90395041322313996</v>
+      </c>
+      <c r="C4">
+        <v>0.73476504358919803</v>
+      </c>
+      <c r="D4">
+        <v>0.91389677112891698</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>0.93430460448642205</v>
+      </c>
+      <c r="H4">
+        <v>0.76070451304582398</v>
+      </c>
+      <c r="I4">
+        <v>0.95854749385101401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.93288547815820499</v>
+      </c>
+      <c r="C5">
+        <v>0.66517802269840598</v>
+      </c>
+      <c r="D5">
+        <v>0.94925744124802902</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>0.94204486422668199</v>
+      </c>
+      <c r="H5">
+        <v>0.71879510123293799</v>
+      </c>
+      <c r="I5">
+        <v>0.97091984490583905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0.94895159386068395</v>
+      </c>
+      <c r="C6">
+        <v>0.37546565583948699</v>
+      </c>
+      <c r="D6">
+        <v>0.99361920905680301</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>0.95828571428571396</v>
+      </c>
+      <c r="H6">
+        <v>0.77356684655330399</v>
+      </c>
+      <c r="I6">
+        <v>0.98251312116881895</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0.92832113341204203</v>
+      </c>
+      <c r="C7">
+        <v>0.62369337979093997</v>
+      </c>
+      <c r="D7">
+        <v>0.96407530044985001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7">
+        <v>0.93754899645808698</v>
+      </c>
+      <c r="H7">
+        <v>0.74582057332195395</v>
+      </c>
+      <c r="I7">
+        <v>0.96904682701797695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>0.89107438016528895</v>
+      </c>
+      <c r="C8">
+        <v>0.499390256505653</v>
+      </c>
+      <c r="D8">
+        <v>0.941591868180497</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8">
+        <v>0.93644155844155796</v>
+      </c>
+      <c r="H8">
+        <v>0.76094767172992706</v>
+      </c>
+      <c r="I8">
+        <v>0.96330572481880195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0.94396221959858295</v>
+      </c>
+      <c r="C9">
+        <v>0.76137933541772695</v>
+      </c>
+      <c r="D9">
+        <v>0.971220229695403</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>0.93096812278630403</v>
+      </c>
+      <c r="H9">
+        <v>0.46865519775395198</v>
+      </c>
+      <c r="I9">
+        <v>0.99720324272667604</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>0.90775914994096796</v>
+      </c>
+      <c r="C10">
+        <v>0.65718921424708299</v>
+      </c>
+      <c r="D10">
+        <v>0.95295511239321595</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10">
+        <v>0.92191971664698902</v>
+      </c>
+      <c r="H10">
+        <v>0.52170816301251</v>
+      </c>
+      <c r="I10">
+        <v>0.993934513925263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0.96025265643447399</v>
+      </c>
+      <c r="C11">
+        <v>0.36726577437858499</v>
+      </c>
+      <c r="D11">
+        <v>0.99927771486095296</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11">
+        <v>0.94220306965761502</v>
+      </c>
+      <c r="H11">
+        <v>0.74579536860301798</v>
+      </c>
+      <c r="I11">
+        <v>0.97184522483055502</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>0.95557497048406104</v>
+      </c>
+      <c r="C12">
+        <v>0.34505850043263903</v>
+      </c>
+      <c r="D12">
+        <v>0.99646023495977698</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0.92881700118063704</v>
+      </c>
+      <c r="C13">
+        <v>0.30538510744154002</v>
+      </c>
+      <c r="D13">
+        <v>0.99783105292283303</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <f>AVERAGE(B3:B13)</f>
+        <v>0.92938757110657899</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:D15" si="0">AVERAGE(C3:C13)</f>
+        <v>0.54381438736671484</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.96635264337769122</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15">
+        <f>AVERAGE(G3:G13)</f>
+        <v>0.93730578512396656</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:I15" si="1">AVERAGE(H3:H13)</f>
+        <v>0.69278581275399909</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0.97445414868112346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <f>MEDIAN(B3:B13)</f>
+        <v>0.92881700118063704</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:D16" si="2">MEDIAN(C3:C13)</f>
+        <v>0.62369337979093997</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>0.96407530044985001</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16">
+        <f>MEDIAN(G3:G13)</f>
+        <v>0.93644155844155796</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:I16" si="3">MEDIAN(H3:H13)</f>
+        <v>0.74579536860301798</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>0.97091984490583905</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <f>_xlfn.STDEV.P(B3:B13)</f>
+        <v>2.1081919113738905E-2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:D17" si="4">_xlfn.STDEV.P(C3:C13)</f>
+        <v>0.16132492055641368</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="4"/>
+        <v>2.6744112207552163E-2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17">
+        <f>_xlfn.STDEV.P(G3:G13)</f>
+        <v>9.4344913526060309E-3</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ref="H17:I17" si="5">_xlfn.STDEV.P(H3:H13)</f>
+        <v>0.10735656532746715</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>1.3014038526537231E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <f>MIN(B3:B13)</f>
+        <v>0.89107438016528895</v>
+      </c>
+      <c r="C18">
+        <f>MIN(C3:C13)</f>
+        <v>0.30538510744154002</v>
+      </c>
+      <c r="D18">
+        <f>MIN(D3:D13)</f>
+        <v>0.91389677112891698</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18">
+        <f>MIN(G3:G13)</f>
+        <v>0.92191971664698902</v>
+      </c>
+      <c r="H18">
+        <f>MIN(H3:H13)</f>
+        <v>0.46865519775395198</v>
+      </c>
+      <c r="I18">
+        <f>MIN(I3:I13)</f>
+        <v>0.95854749385101401</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <f>MAX(B3:B13)</f>
+        <v>0.96025265643447399</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:D19" si="6">MAX(C3:C13)</f>
+        <v>0.76137933541772695</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="6"/>
+        <v>0.99927771486095296</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19">
+        <f>MAX(G3:G13)</f>
+        <v>0.95828571428571396</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ref="H19:I19" si="7">MAX(H3:H13)</f>
+        <v>0.77356684655330399</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="7"/>
+        <v>0.99720324272667604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added preprocessed images, teaks, some comments
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -3,16 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D984F5-3BB6-49D1-80D7-B9479A0364DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EE641C-9731-4BE0-93C8-0300A6DE522F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="c0.6322369" sheetId="1" r:id="rId1"/>
-    <sheet name="HotNewC" sheetId="2" r:id="rId2"/>
+    <sheet name="Stats" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Accuracy</t>
   </si>
@@ -436,11 +434,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64A9E1F-9317-42E7-BDF9-5919A3FD3079}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,25 +482,25 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.92221015348288005</v>
+        <v>0.91743565525383697</v>
       </c>
       <c r="C3">
-        <v>0.62735186745296201</v>
+        <v>0.64718797069260403</v>
       </c>
       <c r="D3">
-        <v>0.95226225447468105</v>
+        <v>0.94497943168483201</v>
       </c>
       <c r="F3" t="s">
         <v>22</v>
       </c>
       <c r="G3">
-        <v>0.94204250295159297</v>
+        <v>0.93203541912632804</v>
       </c>
       <c r="H3">
-        <v>0.66738271180615205</v>
+        <v>0.73907887953256501</v>
       </c>
       <c r="I3">
-        <v>0.98579288823191202</v>
+        <v>0.96277134488516602</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -510,25 +508,25 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.92359858323494604</v>
+        <v>0.90281227863045999</v>
       </c>
       <c r="C4">
-        <v>0.62066765894110099</v>
+        <v>0.73493514777801405</v>
       </c>
       <c r="D4">
-        <v>0.94140780279260405</v>
+        <v>0.91268172556470795</v>
       </c>
       <c r="F4" t="s">
         <v>23</v>
       </c>
       <c r="G4">
-        <v>0.94561983471074296</v>
+        <v>0.93401889020070805</v>
       </c>
       <c r="H4">
-        <v>0.72025667707249397</v>
+        <v>0.76436582263845498</v>
       </c>
       <c r="I4">
-        <v>0.97709132791181996</v>
+        <v>0.95771058594317604</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -536,25 +534,25 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.89229043683589104</v>
+        <v>0.932772136953955</v>
       </c>
       <c r="C5">
-        <v>0.78166099889375995</v>
+        <v>0.66530093825541803</v>
       </c>
       <c r="D5">
-        <v>0.89905610972881</v>
+        <v>0.94912965148474104</v>
       </c>
       <c r="F5" t="s">
         <v>24</v>
       </c>
       <c r="G5">
-        <v>0.94802597402597399</v>
+        <v>0.94161511216056604</v>
       </c>
       <c r="H5">
-        <v>0.72920704300853501</v>
+        <v>0.72543400272153702</v>
       </c>
       <c r="I5">
-        <v>0.97632787374866004</v>
+        <v>0.96957583773780098</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -562,25 +560,25 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.94261393152302198</v>
+        <v>0.94895159386068395</v>
       </c>
       <c r="C6">
-        <v>0.26586497614534998</v>
+        <v>0.37546565583948699</v>
       </c>
       <c r="D6">
-        <v>0.99532448625342895</v>
+        <v>0.99361920905680301</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
       </c>
       <c r="G6">
-        <v>0.96167414403777995</v>
+        <v>0.95886186540731999</v>
       </c>
       <c r="H6">
-        <v>0.76092047652988404</v>
+        <v>0.810243356073719</v>
       </c>
       <c r="I6">
-        <v>0.98800464749796302</v>
+        <v>0.97835441178434501</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -588,25 +586,25 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.92842739079102699</v>
+        <v>0.92775914994096798</v>
       </c>
       <c r="C7">
-        <v>0.74728560188827697</v>
+        <v>0.62522198493874304</v>
       </c>
       <c r="D7">
-        <v>0.94968800707096002</v>
+        <v>0.96326794454045295</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
       </c>
       <c r="G7">
-        <v>0.93940259740259702</v>
+        <v>0.93670365997638705</v>
       </c>
       <c r="H7">
-        <v>0.65711130076810997</v>
+        <v>0.76001137941998398</v>
       </c>
       <c r="I7">
-        <v>0.98577842047819397</v>
+        <v>0.96573129929648105</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -614,25 +612,25 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.90025265643447405</v>
+        <v>0.88751593860684697</v>
       </c>
       <c r="C8">
-        <v>0.525702238482048</v>
+        <v>0.70358198466340005</v>
       </c>
       <c r="D8">
-        <v>0.94856032352400099</v>
+        <v>0.911238833543488</v>
       </c>
       <c r="F8" t="s">
         <v>27</v>
       </c>
       <c r="G8">
-        <v>0.94318299881936196</v>
+        <v>0.93615584415584396</v>
       </c>
       <c r="H8">
-        <v>0.69037031766923895</v>
+        <v>0.77149514424958199</v>
       </c>
       <c r="I8">
-        <v>0.98188293336382704</v>
+        <v>0.96136169332222399</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -640,25 +638,25 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.94714757969303398</v>
+        <v>0.94431404958677601</v>
       </c>
       <c r="C9">
-        <v>0.76179742601614198</v>
+        <v>0.76619646622555004</v>
       </c>
       <c r="D9">
-        <v>0.97481871865569503</v>
+        <v>0.97090542975619198</v>
       </c>
       <c r="F9" t="s">
         <v>28</v>
       </c>
       <c r="G9">
-        <v>0.94747579693034201</v>
+        <v>0.93149704840613901</v>
       </c>
       <c r="H9">
-        <v>0.64671854685232899</v>
+        <v>0.477398202408094</v>
       </c>
       <c r="I9">
-        <v>0.99056499356151895</v>
+        <v>0.99655534528884004</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -666,25 +664,25 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.91389138134592596</v>
+        <v>0.90771664698937404</v>
       </c>
       <c r="C10">
-        <v>0.56515490998995599</v>
+        <v>0.65725102371938504</v>
       </c>
       <c r="D10">
-        <v>0.97679390164025803</v>
+        <v>0.95289379433365295</v>
       </c>
       <c r="F10" t="s">
         <v>29</v>
       </c>
       <c r="G10">
-        <v>0.91023376623376595</v>
+        <v>0.92191971664698902</v>
       </c>
       <c r="H10">
-        <v>0.42146661711879102</v>
+        <v>0.52170816301251</v>
       </c>
       <c r="I10">
-        <v>0.99818341896153895</v>
+        <v>0.993934513925263</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -692,25 +690,25 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.97143801652892503</v>
+        <v>0.96025265643447399</v>
       </c>
       <c r="C11">
-        <v>0.55892925430210305</v>
+        <v>0.36726577437858499</v>
       </c>
       <c r="D11">
-        <v>0.99858562979740695</v>
+        <v>0.99927771486095296</v>
       </c>
       <c r="F11" t="s">
         <v>30</v>
       </c>
       <c r="G11">
-        <v>0.94673671782762603</v>
+        <v>0.94220306965761502</v>
       </c>
       <c r="H11">
-        <v>0.67005798249720805</v>
+        <v>0.74583138257643899</v>
       </c>
       <c r="I11">
-        <v>0.98849350211704301</v>
+        <v>0.97183978954577299</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -718,13 +716,13 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>0.96193388429752003</v>
+        <v>0.95524675324675301</v>
       </c>
       <c r="C12">
-        <v>0.460479289718219</v>
+        <v>0.349422519845002</v>
       </c>
       <c r="D12">
-        <v>0.99551545781381001</v>
+        <v>0.99581778650052</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -732,13 +730,13 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>0.93356552538370696</v>
+        <v>0.92979693034238398</v>
       </c>
       <c r="C13">
-        <v>0.37885285128764001</v>
+        <v>0.31682816460944302</v>
       </c>
       <c r="D13">
-        <v>0.99497234395776402</v>
+        <v>0.99765271144611301</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -747,30 +745,30 @@
       </c>
       <c r="B15">
         <f>AVERAGE(B3:B13)</f>
-        <v>0.93066995814103204</v>
+        <v>0.92859761725877377</v>
       </c>
       <c r="C15">
         <f t="shared" ref="C15:D15" si="0">AVERAGE(C3:C13)</f>
-        <v>0.57215882482886882</v>
+        <v>0.56442342099505738</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>0.96608954870085628</v>
+        <v>0.96286038479749603</v>
       </c>
       <c r="F15" t="s">
         <v>15</v>
       </c>
       <c r="G15">
         <f>AVERAGE(G3:G13)</f>
-        <v>0.9427104814377536</v>
+        <v>0.93722340285976613</v>
       </c>
       <c r="H15">
         <f t="shared" ref="H15:I15" si="1">AVERAGE(H3:H13)</f>
-        <v>0.66261018592474907</v>
+        <v>0.70172959251476508</v>
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
-        <v>0.98579111176360845</v>
+        <v>0.97309275796989647</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -779,30 +777,30 @@
       </c>
       <c r="B16">
         <f>MEDIAN(B3:B13)</f>
-        <v>0.92842739079102699</v>
+        <v>0.92979693034238398</v>
       </c>
       <c r="C16">
         <f t="shared" ref="C16:D16" si="2">MEDIAN(C3:C13)</f>
-        <v>0.56515490998995599</v>
+        <v>0.64718797069260403</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>0.97481871865569503</v>
+        <v>0.96326794454045295</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
       </c>
       <c r="G16">
         <f>MEDIAN(G3:G13)</f>
-        <v>0.94561983471074296</v>
+        <v>0.93615584415584396</v>
       </c>
       <c r="H16">
         <f t="shared" ref="H16:I16" si="3">MEDIAN(H3:H13)</f>
-        <v>0.67005798249720805</v>
+        <v>0.74583138257643899</v>
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
-        <v>0.98579288823191202</v>
+        <v>0.96957583773780098</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -811,30 +809,30 @@
       </c>
       <c r="B17">
         <f>_xlfn.STDEV.P(B3:B13)</f>
-        <v>2.3097313439758946E-2</v>
+        <v>2.1963334903635747E-2</v>
       </c>
       <c r="C17">
         <f t="shared" ref="C17:D17" si="4">_xlfn.STDEV.P(C3:C13)</f>
-        <v>0.15431975583992644</v>
+        <v>0.16530862681296446</v>
       </c>
       <c r="D17">
         <f t="shared" si="4"/>
-        <v>2.9652084580282258E-2</v>
+        <v>3.0783982281232303E-2</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
       </c>
       <c r="G17">
         <f>_xlfn.STDEV.P(G3:G13)</f>
-        <v>1.2916856787873984E-2</v>
+        <v>9.5329550700105955E-3</v>
       </c>
       <c r="H17">
         <f t="shared" ref="H17:I17" si="5">_xlfn.STDEV.P(H3:H13)</f>
-        <v>9.2318919965485885E-2</v>
+        <v>0.11085358559701031</v>
       </c>
       <c r="I17">
         <f t="shared" si="5"/>
-        <v>6.4037750550609649E-3</v>
+        <v>1.3171717130737703E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -843,30 +841,30 @@
       </c>
       <c r="B18">
         <f>MIN(B3:B13)</f>
-        <v>0.89229043683589104</v>
+        <v>0.88751593860684697</v>
       </c>
       <c r="C18">
         <f>MIN(C3:C13)</f>
-        <v>0.26586497614534998</v>
+        <v>0.31682816460944302</v>
       </c>
       <c r="D18">
         <f>MIN(D3:D13)</f>
-        <v>0.89905610972881</v>
+        <v>0.911238833543488</v>
       </c>
       <c r="F18" t="s">
         <v>18</v>
       </c>
       <c r="G18">
         <f>MIN(G3:G13)</f>
-        <v>0.91023376623376595</v>
+        <v>0.92191971664698902</v>
       </c>
       <c r="H18">
         <f>MIN(H3:H13)</f>
-        <v>0.42146661711879102</v>
+        <v>0.477398202408094</v>
       </c>
       <c r="I18">
         <f>MIN(I3:I13)</f>
-        <v>0.97632787374866004</v>
+        <v>0.95771058594317604</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -875,518 +873,11 @@
       </c>
       <c r="B19">
         <f>MAX(B3:B13)</f>
-        <v>0.97143801652892503</v>
+        <v>0.96025265643447399</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:D19" si="6">MAX(C3:C13)</f>
-        <v>0.78166099889375995</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="6"/>
-        <v>0.99858562979740695</v>
-      </c>
-      <c r="F19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19">
-        <f>MAX(G3:G13)</f>
-        <v>0.96167414403777995</v>
-      </c>
-      <c r="H19">
-        <f t="shared" ref="H19:I19" si="7">MAX(H3:H13)</f>
-        <v>0.76092047652988404</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="7"/>
-        <v>0.99818341896153895</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B3:D13">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12:I13">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:I11">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCFA4DA-2F81-4370-BEFA-BFE35C1005F5}">
-  <dimension ref="A1:I19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>0.92171428571428504</v>
-      </c>
-      <c r="C3">
-        <v>0.64718797069260403</v>
-      </c>
-      <c r="D3">
-        <v>0.94969414225832505</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3">
-        <v>0.93203541912632804</v>
-      </c>
-      <c r="H3">
-        <v>0.73907887953256501</v>
-      </c>
-      <c r="I3">
-        <v>0.96277134488516602</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>0.90395041322313996</v>
-      </c>
-      <c r="C4">
-        <v>0.73476504358919803</v>
-      </c>
-      <c r="D4">
-        <v>0.91389677112891698</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4">
-        <v>0.93430460448642205</v>
-      </c>
-      <c r="H4">
-        <v>0.76070451304582398</v>
-      </c>
-      <c r="I4">
-        <v>0.95854749385101401</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.93288547815820499</v>
-      </c>
-      <c r="C5">
-        <v>0.66517802269840598</v>
-      </c>
-      <c r="D5">
-        <v>0.94925744124802902</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5">
-        <v>0.94204486422668199</v>
-      </c>
-      <c r="H5">
-        <v>0.71879510123293799</v>
-      </c>
-      <c r="I5">
-        <v>0.97091984490583905</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>0.94895159386068395</v>
-      </c>
-      <c r="C6">
-        <v>0.37546565583948699</v>
-      </c>
-      <c r="D6">
-        <v>0.99361920905680301</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6">
-        <v>0.95828571428571396</v>
-      </c>
-      <c r="H6">
-        <v>0.77356684655330399</v>
-      </c>
-      <c r="I6">
-        <v>0.98251312116881895</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0.92832113341204203</v>
-      </c>
-      <c r="C7">
-        <v>0.62369337979093997</v>
-      </c>
-      <c r="D7">
-        <v>0.96407530044985001</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7">
-        <v>0.93754899645808698</v>
-      </c>
-      <c r="H7">
-        <v>0.74582057332195395</v>
-      </c>
-      <c r="I7">
-        <v>0.96904682701797695</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>0.89107438016528895</v>
-      </c>
-      <c r="C8">
-        <v>0.499390256505653</v>
-      </c>
-      <c r="D8">
-        <v>0.941591868180497</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8">
-        <v>0.93644155844155796</v>
-      </c>
-      <c r="H8">
-        <v>0.76094767172992706</v>
-      </c>
-      <c r="I8">
-        <v>0.96330572481880195</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0.94396221959858295</v>
-      </c>
-      <c r="C9">
-        <v>0.76137933541772695</v>
-      </c>
-      <c r="D9">
-        <v>0.971220229695403</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9">
-        <v>0.93096812278630403</v>
-      </c>
-      <c r="H9">
-        <v>0.46865519775395198</v>
-      </c>
-      <c r="I9">
-        <v>0.99720324272667604</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>0.90775914994096796</v>
-      </c>
-      <c r="C10">
-        <v>0.65718921424708299</v>
-      </c>
-      <c r="D10">
-        <v>0.95295511239321595</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>0.92191971664698902</v>
-      </c>
-      <c r="H10">
-        <v>0.52170816301251</v>
-      </c>
-      <c r="I10">
-        <v>0.993934513925263</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>0.96025265643447399</v>
-      </c>
-      <c r="C11">
-        <v>0.36726577437858499</v>
-      </c>
-      <c r="D11">
-        <v>0.99927771486095296</v>
-      </c>
-      <c r="F11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11">
-        <v>0.94220306965761502</v>
-      </c>
-      <c r="H11">
-        <v>0.74579536860301798</v>
-      </c>
-      <c r="I11">
-        <v>0.97184522483055502</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>0.95557497048406104</v>
-      </c>
-      <c r="C12">
-        <v>0.34505850043263903</v>
-      </c>
-      <c r="D12">
-        <v>0.99646023495977698</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>0.92881700118063704</v>
-      </c>
-      <c r="C13">
-        <v>0.30538510744154002</v>
-      </c>
-      <c r="D13">
-        <v>0.99783105292283303</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <f>AVERAGE(B3:B13)</f>
-        <v>0.92938757110657899</v>
-      </c>
-      <c r="C15">
-        <f t="shared" ref="C15:D15" si="0">AVERAGE(C3:C13)</f>
-        <v>0.54381438736671484</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0.96635264337769122</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15">
-        <f>AVERAGE(G3:G13)</f>
-        <v>0.93730578512396656</v>
-      </c>
-      <c r="H15">
-        <f t="shared" ref="H15:I15" si="1">AVERAGE(H3:H13)</f>
-        <v>0.69278581275399909</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>0.97445414868112346</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <f>MEDIAN(B3:B13)</f>
-        <v>0.92881700118063704</v>
-      </c>
-      <c r="C16">
-        <f t="shared" ref="C16:D16" si="2">MEDIAN(C3:C13)</f>
-        <v>0.62369337979093997</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="2"/>
-        <v>0.96407530044985001</v>
-      </c>
-      <c r="F16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16">
-        <f>MEDIAN(G3:G13)</f>
-        <v>0.93644155844155796</v>
-      </c>
-      <c r="H16">
-        <f t="shared" ref="H16:I16" si="3">MEDIAN(H3:H13)</f>
-        <v>0.74579536860301798</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="3"/>
-        <v>0.97091984490583905</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <f>_xlfn.STDEV.P(B3:B13)</f>
-        <v>2.1081919113738905E-2</v>
-      </c>
-      <c r="C17">
-        <f t="shared" ref="C17:D17" si="4">_xlfn.STDEV.P(C3:C13)</f>
-        <v>0.16132492055641368</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="4"/>
-        <v>2.6744112207552163E-2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17">
-        <f>_xlfn.STDEV.P(G3:G13)</f>
-        <v>9.4344913526060309E-3</v>
-      </c>
-      <c r="H17">
-        <f t="shared" ref="H17:I17" si="5">_xlfn.STDEV.P(H3:H13)</f>
-        <v>0.10735656532746715</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="5"/>
-        <v>1.3014038526537231E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <f>MIN(B3:B13)</f>
-        <v>0.89107438016528895</v>
-      </c>
-      <c r="C18">
-        <f>MIN(C3:C13)</f>
-        <v>0.30538510744154002</v>
-      </c>
-      <c r="D18">
-        <f>MIN(D3:D13)</f>
-        <v>0.91389677112891698</v>
-      </c>
-      <c r="F18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18">
-        <f>MIN(G3:G13)</f>
-        <v>0.92191971664698902</v>
-      </c>
-      <c r="H18">
-        <f>MIN(H3:H13)</f>
-        <v>0.46865519775395198</v>
-      </c>
-      <c r="I18">
-        <f>MIN(I3:I13)</f>
-        <v>0.95854749385101401</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <f>MAX(B3:B13)</f>
-        <v>0.96025265643447399</v>
-      </c>
-      <c r="C19">
-        <f t="shared" ref="C19:D19" si="6">MAX(C3:C13)</f>
-        <v>0.76137933541772695</v>
+        <v>0.76619646622555004</v>
       </c>
       <c r="D19">
         <f t="shared" si="6"/>
@@ -1397,15 +888,15 @@
       </c>
       <c r="G19">
         <f>MAX(G3:G13)</f>
-        <v>0.95828571428571396</v>
+        <v>0.95886186540731999</v>
       </c>
       <c r="H19">
         <f t="shared" ref="H19:I19" si="7">MAX(H3:H13)</f>
-        <v>0.77356684655330399</v>
+        <v>0.810243356073719</v>
       </c>
       <c r="I19">
         <f t="shared" si="7"/>
-        <v>0.99720324272667604</v>
+        <v>0.99655534528884004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>